<commit_message>
Added Edit Product Functionality
</commit_message>
<xml_diff>
--- a/data/all_store_data.xlsx
+++ b/data/all_store_data.xlsx
@@ -3,32 +3,80 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OnlineStoreApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76271B52-45F1-4AF2-A2FC-CDF285D24A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B34DC0-E08D-4200-9E80-8B8B815797A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3684" yWindow="804" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="4" r:id="rId1"/>
-    <sheet name="Customers" sheetId="5" r:id="rId2"/>
+    <sheet name="Products" sheetId="6" r:id="rId1"/>
+    <sheet name="Customers" r:id="rId5" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>P#00001</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>P#005</t>
+  </si>
+  <si>
+    <t>T-Shirt</t>
+  </si>
+  <si>
+    <t>Levis</t>
+  </si>
+  <si>
+    <t>P#00002</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>I Phone</t>
+  </si>
+  <si>
+    <t>P#00003</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
+    <t>Writometer</t>
+  </si>
   <si>
     <t>CustomerId</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -38,76 +86,20 @@
     <t>C#00001</t>
   </si>
   <si>
-    <t>ProductId</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>P#00001</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>SMart Phone</t>
-  </si>
-  <si>
-    <t>P#00002</t>
-  </si>
-  <si>
-    <t>Shelf</t>
-  </si>
-  <si>
-    <t>Book Shelf Wood</t>
-  </si>
-  <si>
-    <t>Raj</t>
-  </si>
-  <si>
-    <t>raj@gmail.com</t>
-  </si>
-  <si>
-    <t>raj</t>
-  </si>
-  <si>
-    <t>P#00003</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>P#00004</t>
-  </si>
-  <si>
-    <t>Pen</t>
-  </si>
-  <si>
-    <t>Writometer</t>
-  </si>
-  <si>
-    <t>Pencil</t>
-  </si>
-  <si>
-    <t>P#0001</t>
-  </si>
-  <si>
-    <t>Apsara</t>
+    <t>Lucky</t>
+  </si>
+  <si>
+    <t>lucky@gmail.com</t>
+  </si>
+  <si>
+    <t>lucky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,118 +444,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>12.55</v>
+        <v>580.25</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>4555.99</v>
+        <v>1622.99</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>589.65</v>
+        <v>650000</v>
       </c>
       <c r="E4">
-        <v>11.22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>-8</v>
-      </c>
-      <c r="E6">
-        <v>25.22</v>
+        <v>21.25</v>
       </c>
     </row>
   </sheetData>
@@ -571,43 +543,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creating fiel export directory if not exists
</commit_message>
<xml_diff>
--- a/data/all_store_data.xlsx
+++ b/data/all_store_data.xlsx
@@ -10,18 +10,18 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B34DC0-E08D-4200-9E80-8B8B815797A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="804" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3684" yWindow="804" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="6" r:id="rId1"/>
     <sheet name="Customers" r:id="rId5" sheetId="7"/>
+    <sheet name="Products" r:id="rId6" sheetId="8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -443,106 +443,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>580.25</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>1622.99</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>650000</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>21.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D1"/>
@@ -568,4 +468,34 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Excel Cell Type Validations
</commit_message>
<xml_diff>
--- a/data/all_store_data.xlsx
+++ b/data/all_store_data.xlsx
@@ -3,25 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OnlineStoreApp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B34DC0-E08D-4200-9E80-8B8B815797A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A8CDE1-9A1A-4D4A-9B24-18A3DA4605D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="804" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="3684" yWindow="804" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" r:id="rId5" sheetId="7"/>
-    <sheet name="Products" r:id="rId6" sheetId="8"/>
+    <sheet name="Products" sheetId="6" r:id="rId1"/>
+    <sheet name="Customers" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>java</t>
   </si>
   <si>
-    <t>P#005</t>
-  </si>
-  <si>
     <t>T-Shirt</t>
   </si>
   <si>
@@ -86,24 +83,64 @@
     <t>C#00001</t>
   </si>
   <si>
-    <t>Lucky</t>
-  </si>
-  <si>
-    <t>lucky@gmail.com</t>
-  </si>
-  <si>
-    <t>lucky</t>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>raj@gmail.com</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>P#00004</t>
+  </si>
+  <si>
+    <t>P#00005</t>
+  </si>
+  <si>
+    <t>Abcd</t>
+  </si>
+  <si>
+    <t>P#00006</t>
+  </si>
+  <si>
+    <t>P#00007</t>
+  </si>
+  <si>
+    <t>P#00008</t>
+  </si>
+  <si>
+    <t>P#00009</t>
+  </si>
+  <si>
+    <t>C#00002</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>aman@gmail.com</t>
+  </si>
+  <si>
+    <t>C#00003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,13 +163,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,59 +483,305 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64996B2-ECB1-4166-A8E2-A8910C35AA93}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>580.25</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1622.99</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>650000</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>-25600</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>650000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>650000</v>
+      </c>
+      <c r="E11">
+        <v>25.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>650000</v>
+      </c>
+      <c r="E12">
+        <v>-25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E64BD4-7E14-4ADD-9E39-77EEA90CDB49}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1234</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{34BDC3BE-2C59-47EA-B1E5-5CDDE9BEFE60}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1E966601-5E2C-43F0-898B-D53F0CE8EC2D}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{B1A8BEB8-9562-4F56-A410-1FF832E33F53}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>